<commit_message>
Committ out vlidation xls
</commit_message>
<xml_diff>
--- a/lib/ValidationData.xlsx
+++ b/lib/ValidationData.xlsx
@@ -1,22 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\MechEng\ResearchProjects\DCleaver\KA-ME1DJC\Teaching\ME40343 Helicopters\Coursework\Moodle\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\Documents\GitProjects\Heli\WindTurbineDesign\lib\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB3665FE-40E2-4370-AE5F-B9A9083AE170}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="11475" windowHeight="5190" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="11475" windowHeight="5190" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WTInducedCalcCheck" sheetId="4" r:id="rId1"/>
     <sheet name="WTSingleVelocityCheck" sheetId="1" r:id="rId2"/>
     <sheet name="WTVelocityRangeCheck" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -98,7 +106,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -198,6 +206,9 @@
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -213,9 +224,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1558,7 +1566,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2021,7 +2028,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2053,7 +2059,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -2085,7 +2097,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -2122,7 +2140,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2157,7 +2181,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2187,7 +2217,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -2283,6 +2319,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2318,6 +2371,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2493,54 +2563,54 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P31"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M29" sqref="L11:M29"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="S9" sqref="S9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
-      <c r="O1" s="11"/>
-      <c r="P1" s="11"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13"/>
-      <c r="M2" s="13"/>
-      <c r="N2" s="13"/>
-      <c r="O2" s="13"/>
-      <c r="P2" s="13"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
+      <c r="M2" s="16"/>
+      <c r="N2" s="16"/>
+      <c r="O2" s="16"/>
+      <c r="P2" s="16"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
@@ -2588,44 +2658,44 @@
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="11"/>
-      <c r="L6" s="11"/>
-      <c r="M6" s="11"/>
-      <c r="N6" s="11"/>
-      <c r="O6" s="11"/>
-      <c r="P6" s="11"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="14"/>
+      <c r="O6" s="14"/>
+      <c r="P6" s="14"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="12"/>
-      <c r="L7" s="12"/>
-      <c r="M7" s="12"/>
-      <c r="N7" s="12"/>
-      <c r="O7" s="12"/>
-      <c r="P7" s="12"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="15"/>
+      <c r="N7" s="15"/>
+      <c r="O7" s="15"/>
+      <c r="P7" s="15"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
@@ -2646,26 +2716,26 @@
       <c r="P8" s="5"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
-      <c r="K9" s="14" t="s">
+      <c r="K9" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="L9" s="14"/>
-      <c r="M9" s="14"/>
-      <c r="N9" s="14"/>
-      <c r="O9" s="14"/>
-      <c r="P9" s="14"/>
+      <c r="L9" s="17"/>
+      <c r="M9" s="17"/>
+      <c r="N9" s="17"/>
+      <c r="O9" s="17"/>
+      <c r="P9" s="17"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
@@ -3169,7 +3239,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P26"/>
   <sheetViews>
     <sheetView topLeftCell="A24" workbookViewId="0">
@@ -3183,54 +3253,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
-      <c r="O1" s="11"/>
-      <c r="P1" s="11"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
-      <c r="O2" s="12"/>
-      <c r="P2" s="12"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="15"/>
+      <c r="P2" s="15"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="13"/>
-      <c r="K3" s="13" t="s">
+      <c r="B3" s="16"/>
+      <c r="K3" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="L3" s="13"/>
+      <c r="L3" s="16"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
@@ -3450,11 +3520,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AA27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3471,61 +3541,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
-      <c r="O1" s="11"/>
-      <c r="P1" s="11"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13"/>
-      <c r="M2" s="13"/>
-      <c r="N2" s="13"/>
-      <c r="O2" s="13"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
+      <c r="M2" s="16"/>
+      <c r="N2" s="16"/>
+      <c r="O2" s="16"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="K3" s="15" t="s">
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="K3" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="L3" s="15"/>
-      <c r="M3" s="15"/>
-      <c r="N3" s="15"/>
-      <c r="O3" s="15"/>
-      <c r="P3" s="15"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="18"/>
+      <c r="N3" s="18"/>
+      <c r="O3" s="18"/>
+      <c r="P3" s="18"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
@@ -3566,22 +3636,22 @@
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="16">
+      <c r="A5" s="11">
         <v>5.5</v>
       </c>
-      <c r="B5" s="17">
+      <c r="B5" s="12">
         <v>11082.220890479201</v>
       </c>
-      <c r="C5" s="17">
+      <c r="C5" s="12">
         <v>61947.5529174521</v>
       </c>
-      <c r="D5" s="18">
+      <c r="D5" s="13">
         <v>0.11068015974965301</v>
       </c>
-      <c r="E5" s="17">
+      <c r="E5" s="12">
         <v>10744858.132003199</v>
       </c>
-      <c r="F5" s="17">
+      <c r="F5" s="12">
         <v>60061757.864312001</v>
       </c>
       <c r="K5" s="9"/>
@@ -3592,22 +3662,22 @@
       <c r="P5" s="9"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="16">
+      <c r="A6" s="11">
         <v>6.5</v>
       </c>
-      <c r="B6" s="17">
+      <c r="B6" s="12">
         <v>41733.484761313397</v>
       </c>
-      <c r="C6" s="17">
+      <c r="C6" s="12">
         <v>102253.02311017401</v>
       </c>
-      <c r="D6" s="18">
+      <c r="D6" s="13">
         <v>0.100865090269768</v>
       </c>
-      <c r="E6" s="17">
+      <c r="E6" s="12">
         <v>36874796.959643602</v>
       </c>
-      <c r="F6" s="17">
+      <c r="F6" s="12">
         <v>90348541.159752399</v>
       </c>
       <c r="K6" s="9"/>
@@ -3618,22 +3688,22 @@
       <c r="P6" s="9"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="16">
+      <c r="A7" s="11">
         <v>7.5</v>
       </c>
-      <c r="B7" s="17">
+      <c r="B7" s="12">
         <v>82294.881853811195</v>
       </c>
-      <c r="C7" s="17">
+      <c r="C7" s="12">
         <v>157079.63267948999</v>
       </c>
-      <c r="D7" s="18">
+      <c r="D7" s="13">
         <v>8.7525511639071296E-2</v>
       </c>
-      <c r="E7" s="17">
+      <c r="E7" s="12">
         <v>63097418.362298101</v>
       </c>
-      <c r="F7" s="17">
+      <c r="F7" s="12">
         <v>120436642.912744</v>
       </c>
       <c r="K7" s="9"/>
@@ -3644,22 +3714,22 @@
       <c r="P7" s="9"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="16">
+      <c r="A8" s="11">
         <v>8.5</v>
       </c>
-      <c r="B8" s="17">
+      <c r="B8" s="12">
         <v>131736.58962605201</v>
       </c>
-      <c r="C8" s="17">
+      <c r="C8" s="12">
         <v>228661.40306795001</v>
       </c>
-      <c r="D8" s="18">
+      <c r="D8" s="13">
         <v>7.2730060767989796E-2</v>
       </c>
-      <c r="E8" s="17">
+      <c r="E8" s="12">
         <v>83931401.079305604</v>
       </c>
-      <c r="F8" s="17">
+      <c r="F8" s="12">
         <v>145683685.80612999</v>
       </c>
       <c r="K8" s="9"/>
@@ -3670,22 +3740,22 @@
       <c r="P8" s="9"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="16">
+      <c r="A9" s="11">
         <v>9.5</v>
       </c>
-      <c r="B9" s="17">
+      <c r="B9" s="12">
         <v>186961.13923568901</v>
       </c>
-      <c r="C9" s="17">
+      <c r="C9" s="12">
         <v>319232.355718109</v>
       </c>
-      <c r="D9" s="18">
+      <c r="D9" s="13">
         <v>5.81010029376611E-2</v>
       </c>
-      <c r="E9" s="17">
+      <c r="E9" s="12">
         <v>95156636.171660498</v>
       </c>
-      <c r="F9" s="17">
+      <c r="F9" s="12">
         <v>162478027.527399</v>
       </c>
       <c r="K9" s="9"/>
@@ -3696,22 +3766,22 @@
       <c r="P9" s="9"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="16">
+      <c r="A10" s="11">
         <v>10.5</v>
       </c>
-      <c r="B10" s="17">
+      <c r="B10" s="12">
         <v>250690.25476569001</v>
       </c>
-      <c r="C10" s="17">
+      <c r="C10" s="12">
         <v>431026.51207251998</v>
       </c>
-      <c r="D10" s="18">
+      <c r="D10" s="13">
         <v>4.4749389778345798E-2</v>
       </c>
-      <c r="E10" s="17">
+      <c r="E10" s="12">
         <v>98271746.695489794</v>
       </c>
-      <c r="F10" s="17">
+      <c r="F10" s="12">
         <v>168964398.927358</v>
       </c>
       <c r="K10" s="9"/>
@@ -3722,22 +3792,22 @@
       <c r="P10" s="9"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="16">
+      <c r="A11" s="11">
         <v>11.5</v>
       </c>
-      <c r="B11" s="17">
+      <c r="B11" s="12">
         <v>321217.634918847</v>
       </c>
-      <c r="C11" s="17">
+      <c r="C11" s="12">
         <v>566277.89357373398</v>
       </c>
-      <c r="D11" s="18">
+      <c r="D11" s="13">
         <v>3.3301902577265299E-2</v>
       </c>
-      <c r="E11" s="17">
+      <c r="E11" s="12">
         <v>93707107.445303097</v>
       </c>
-      <c r="F11" s="17">
+      <c r="F11" s="12">
         <v>165197229.692635</v>
       </c>
       <c r="K11" s="9"/>
@@ -3748,22 +3818,22 @@
       <c r="P11" s="9"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="16">
+      <c r="A12" s="11">
         <v>12.5</v>
       </c>
-      <c r="B12" s="17">
+      <c r="B12" s="12">
         <v>397575.10375054402</v>
       </c>
-      <c r="C12" s="17">
+      <c r="C12" s="12">
         <v>727220.52166430396</v>
       </c>
-      <c r="D12" s="18">
+      <c r="D12" s="13">
         <v>2.3986723148667E-2</v>
       </c>
-      <c r="E12" s="17">
+      <c r="E12" s="12">
         <v>83539949.753529698</v>
       </c>
-      <c r="F12" s="17">
+      <c r="F12" s="12">
         <v>152806262.93363199</v>
       </c>
       <c r="K12" s="9"/>
@@ -3774,22 +3844,22 @@
       <c r="P12" s="9"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="16">
+      <c r="A13" s="11">
         <v>13.5</v>
       </c>
-      <c r="B13" s="17">
+      <c r="B13" s="12">
         <v>478750.22153177101</v>
       </c>
-      <c r="C13" s="17">
+      <c r="C13" s="12">
         <v>916088.417786784</v>
       </c>
-      <c r="D13" s="18">
+      <c r="D13" s="13">
         <v>1.67452103568295E-2</v>
       </c>
-      <c r="E13" s="17">
+      <c r="E13" s="12">
         <v>70226932.951051295</v>
       </c>
-      <c r="F13" s="17">
+      <c r="F13" s="12">
         <v>134379216.96894199</v>
       </c>
       <c r="K13" s="9"/>
@@ -3800,22 +3870,22 @@
       <c r="P13" s="9"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="16">
+      <c r="A14" s="11">
         <v>14.5</v>
       </c>
-      <c r="B14" s="17">
+      <c r="B14" s="12">
         <v>559916.45550766401</v>
       </c>
-      <c r="C14" s="17">
+      <c r="C14" s="12">
         <v>1135115.6033837299</v>
       </c>
-      <c r="D14" s="18">
+      <c r="D14" s="13">
         <v>1.13428188707436E-2</v>
       </c>
-      <c r="E14" s="17">
+      <c r="E14" s="12">
         <v>55635031.013132699</v>
       </c>
-      <c r="F14" s="17">
+      <c r="F14" s="12">
         <v>112788597.61406</v>
       </c>
       <c r="K14" s="9"/>
@@ -3826,22 +3896,22 @@
       <c r="P14" s="9"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="16">
+      <c r="A15" s="11">
         <v>15.5</v>
       </c>
-      <c r="B15" s="17">
+      <c r="B15" s="12">
         <v>638004.14921342896</v>
       </c>
-      <c r="C15" s="17">
+      <c r="C15" s="12">
         <v>1386536.0998976801</v>
       </c>
-      <c r="D15" s="18">
+      <c r="D15" s="13">
         <v>7.4623591449101898E-3</v>
       </c>
-      <c r="E15" s="17">
+      <c r="E15" s="12">
         <v>41706501.0129916</v>
       </c>
-      <c r="F15" s="17">
+      <c r="F15" s="12">
         <v>90638233.820619404</v>
       </c>
       <c r="K15" s="9"/>
@@ -3852,22 +3922,22 @@
       <c r="P15" s="9"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="16">
+      <c r="A16" s="11">
         <v>16.5</v>
       </c>
-      <c r="B16" s="17">
+      <c r="B16" s="12">
         <v>709748.37077522394</v>
       </c>
-      <c r="C16" s="17">
+      <c r="C16" s="12">
         <v>1672583.9287712099</v>
       </c>
-      <c r="D16" s="18">
+      <c r="D16" s="13">
         <v>4.7720994397246301E-3</v>
       </c>
-      <c r="E16" s="17">
+      <c r="E16" s="12">
         <v>29670030.670091901</v>
       </c>
-      <c r="F16" s="17">
+      <c r="F16" s="12">
         <v>69920014.625381798</v>
       </c>
       <c r="K16" s="9"/>
@@ -3878,22 +3948,22 @@
       <c r="P16" s="9"/>
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A17" s="16">
+      <c r="A17" s="11">
         <v>17.5</v>
       </c>
-      <c r="B17" s="17">
+      <c r="B17" s="12">
         <v>770569.075954161</v>
       </c>
-      <c r="C17" s="17">
+      <c r="C17" s="12">
         <v>1995493.11144685</v>
       </c>
-      <c r="D17" s="18">
+      <c r="D17" s="13">
         <v>2.9684303285226199E-3</v>
       </c>
-      <c r="E17" s="17">
+      <c r="E17" s="12">
         <v>20037454.189887699</v>
       </c>
-      <c r="F17" s="17">
+      <c r="F17" s="12">
         <v>51889704.706020698</v>
       </c>
       <c r="K17" s="9"/>
@@ -3904,22 +3974,22 @@
       <c r="P17" s="9"/>
     </row>
     <row r="18" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A18" s="16">
+      <c r="A18" s="11">
         <v>18.5</v>
       </c>
-      <c r="B18" s="17">
+      <c r="B18" s="12">
         <v>816655.93169255299</v>
       </c>
-      <c r="C18" s="17">
+      <c r="C18" s="12">
         <v>2357497.66936717</v>
       </c>
-      <c r="D18" s="18">
+      <c r="D18" s="13">
         <v>1.7971987782490701E-3</v>
       </c>
-      <c r="E18" s="17">
+      <c r="E18" s="12">
         <v>12856991.0539444</v>
       </c>
-      <c r="F18" s="17">
+      <c r="F18" s="12">
         <v>37115173.316538498</v>
       </c>
       <c r="K18" s="9"/>
@@ -3930,22 +4000,22 @@
       <c r="P18" s="9"/>
     </row>
     <row r="19" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A19" s="16">
+      <c r="A19" s="11">
         <v>19.5</v>
       </c>
-      <c r="B19" s="17">
+      <c r="B19" s="12">
         <v>843567.15161122102</v>
       </c>
-      <c r="C19" s="17">
+      <c r="C19" s="12">
         <v>2760831.6239747098</v>
       </c>
-      <c r="D19" s="18">
+      <c r="D19" s="13">
         <v>1.0596300187325899E-3</v>
       </c>
-      <c r="E19" s="17">
+      <c r="E19" s="12">
         <v>7830293.1115765702</v>
       </c>
-      <c r="F19" s="17">
+      <c r="F19" s="12">
         <v>25627030.1731654</v>
       </c>
       <c r="K19" s="9"/>
@@ -3956,22 +4026,22 @@
       <c r="P19" s="9"/>
     </row>
     <row r="20" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A20" s="16">
+      <c r="A20" s="11">
         <v>20.5</v>
       </c>
-      <c r="B20" s="17">
+      <c r="B20" s="12">
         <v>855869.38882472797</v>
       </c>
-      <c r="C20" s="17">
+      <c r="C20" s="12">
         <v>3207728.9967120299</v>
       </c>
-      <c r="D20" s="18">
+      <c r="D20" s="13">
         <v>6.0871346989075802E-4</v>
       </c>
-      <c r="E20" s="17">
+      <c r="E20" s="12">
         <v>4563778.0148962904</v>
       </c>
-      <c r="F20" s="17">
+      <c r="F20" s="12">
         <v>17104669.5489861</v>
       </c>
       <c r="K20" s="9"/>
@@ -3982,22 +4052,22 @@
       <c r="P20" s="9"/>
     </row>
     <row r="21" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A21" s="16">
+      <c r="A21" s="11">
         <v>21.5</v>
       </c>
-      <c r="B21" s="17">
+      <c r="B21" s="12">
         <v>844734.32815885497</v>
       </c>
-      <c r="C21" s="17">
+      <c r="C21" s="12">
         <v>3700423.8090216802</v>
       </c>
-      <c r="D21" s="18">
+      <c r="D21" s="13">
         <v>3.4084945285830002E-4</v>
       </c>
-      <c r="E21" s="17">
+      <c r="E21" s="12">
         <v>2522242.5660168701</v>
       </c>
-      <c r="F21" s="17">
+      <c r="F21" s="12">
         <v>11048877.892484101</v>
       </c>
       <c r="K21" s="9"/>
@@ -4008,22 +4078,22 @@
       <c r="P21" s="9"/>
     </row>
     <row r="22" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A22" s="16">
+      <c r="A22" s="11">
         <v>22.5</v>
       </c>
-      <c r="B22" s="17">
+      <c r="B22" s="12">
         <v>800588.31296659005</v>
       </c>
-      <c r="C22" s="17">
+      <c r="C22" s="12">
         <v>4241150.0823462196</v>
       </c>
-      <c r="D22" s="18">
+      <c r="D22" s="13">
         <v>1.8611271272152199E-4</v>
       </c>
-      <c r="E22" s="17">
+      <c r="E22" s="12">
         <v>1305237.0452463799</v>
       </c>
-      <c r="F22" s="17">
+      <c r="F22" s="12">
         <v>6914547.8547087498</v>
       </c>
       <c r="K22" s="9"/>
@@ -4034,22 +4104,22 @@
       <c r="P22" s="9"/>
     </row>
     <row r="23" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A23" s="16">
+      <c r="A23" s="11">
         <v>23.5</v>
       </c>
-      <c r="B23" s="17">
+      <c r="B23" s="12">
         <v>753909.20100765896</v>
       </c>
-      <c r="C23" s="17">
+      <c r="C23" s="12">
         <v>4832141.8381281896</v>
       </c>
-      <c r="D23" s="18">
+      <c r="D23" s="13">
         <v>9.9131303091395403E-5</v>
       </c>
-      <c r="E23" s="17">
+      <c r="E23" s="12">
         <v>654687.37321430305</v>
       </c>
-      <c r="F23" s="17">
+      <c r="F23" s="12">
         <v>4196184.6901122201</v>
       </c>
       <c r="K23" s="9"/>
@@ -4060,22 +4130,22 @@
       <c r="P23" s="9"/>
     </row>
     <row r="24" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A24" s="16">
+      <c r="A24" s="11">
         <v>24.5</v>
       </c>
-      <c r="B24" s="17">
+      <c r="B24" s="12">
         <v>746834.37975413399</v>
       </c>
-      <c r="C24" s="17">
+      <c r="C24" s="12">
         <v>5475633.0978101604</v>
       </c>
-      <c r="D24" s="18">
+      <c r="D24" s="13">
         <v>5.1524232670873199E-5</v>
       </c>
-      <c r="E24" s="17">
+      <c r="E24" s="12">
         <v>337085.39873775898</v>
       </c>
-      <c r="F24" s="17">
+      <c r="F24" s="12">
         <v>2471439.47326669</v>
       </c>
       <c r="K24" s="9"/>

</xml_diff>